<commit_message>
No more EnumValue import from python-docx
</commit_message>
<xml_diff>
--- a/tests/comments.xlsx
+++ b/tests/comments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djslo\Documents\Code\daniel-sloat\comment-response\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsloat\Code\comment-response\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE0F99-3F28-426E-9E67-07D759014794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E691E-5D1F-48C3-8532-1DB7C6B1F700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="84">
   <si>
     <t>Comment Number</t>
   </si>
@@ -2344,9 +2344,6 @@
   </si>
   <si>
     <t>Subsubgroup 1</t>
-  </si>
-  <si>
-    <t>Subsubgroup 2</t>
   </si>
   <si>
     <t>Oops second response</t>
@@ -2559,9 +2556,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2599,9 +2596,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2634,26 +2631,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2686,26 +2666,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2881,26 +2844,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.68359375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.68359375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.68359375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.68359375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.68359375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.68359375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.68359375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.68359375" style="3" customWidth="1"/>
-    <col min="9" max="12" width="18.68359375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="80.68359375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" style="3" customWidth="1"/>
+    <col min="9" max="12" width="18.6328125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="80.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2944,7 +2907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2982,7 +2945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -3020,7 +2983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="62.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>9</v>
       </c>
@@ -3058,7 +3021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="173.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="186" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>15</v>
       </c>
@@ -3099,7 +3062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>20</v>
       </c>
@@ -3134,16 +3097,16 @@
         <v>80</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="261" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -3178,7 +3141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3213,7 +3176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="109.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" ht="124" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>10</v>
       </c>
@@ -3248,7 +3211,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>16</v>
       </c>
@@ -3283,7 +3246,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -3318,7 +3281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -3353,7 +3316,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3388,7 +3351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>17</v>
       </c>
@@ -3423,7 +3386,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -3458,7 +3421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -3493,7 +3456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -3528,7 +3491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -3563,7 +3526,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -3601,7 +3564,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3642,7 +3605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="90.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" ht="91" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -3677,7 +3640,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" ht="116" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3715,7 +3678,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -3750,7 +3713,7 @@
         <v>78</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise column name ('commenter code" to "document code")
</commit_message>
<xml_diff>
--- a/tests/comments.xlsx
+++ b/tests/comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsloat\Code\comment-response\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E691E-5D1F-48C3-8532-1DB7C6B1F700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEACC47-3072-4DBF-9A90-AFC97642E225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comments" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>Document Number</t>
   </si>
   <si>
-    <t>Commenter Code</t>
-  </si>
-  <si>
     <t>Document Comment Number</t>
   </si>
   <si>
@@ -2352,6 +2349,9 @@
     <t>Paragraph
 Paragraph 2
 Paragraph 3</t>
+  </si>
+  <si>
+    <t>Document Code</t>
   </si>
 </sst>
 </file>
@@ -2844,26 +2844,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" style="3" customWidth="1"/>
-    <col min="9" max="12" width="18.6328125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="80.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="3" customWidth="1"/>
+    <col min="9" max="12" width="18.6640625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="80.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2874,846 +2874,846 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="186" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="171" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>104</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="3">
         <v>44701.657638888893</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>82</v>
-      </c>
     </row>
-    <row r="7" spans="1:14" ht="261" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1">
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="124" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="106.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1">
         <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
         <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>100</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1">
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>101</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>103</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
         <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1">
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>101</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1">
         <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>103</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1">
         <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1">
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>104</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="3">
         <v>44701.656944444447</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="91" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="90" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1">
         <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="M21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1">
         <v>104</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="3">
         <v>44701.665277777778</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1">
         <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="3">
         <v>44701.665277777778</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>